<commit_message>
- Adjusted T4 size and drilling holes on footprint - Changed footprint of the TTGO T4 expansion connector to match pn numbering of schematic. - Signals on the TTGO T4 were mirrorred top bottom, corrected order. - TTGO-T4 to Wemos mapping was not followed making most Dx signals on the inner Wemos connector unusable. - Added jumpers to replace I2C by other signals. Cut them if you want to use the I2C connector on the board. - Added ground planes at both sides. Board is now 2 layers. - Used proper drill holes. The mounting holes did not appear in a drilling file. Not a clue if they can be done as an edge cut. But this will certainly work.\ - Lots of small changes hre and there.
</commit_message>
<xml_diff>
--- a/wemos-baseplate/wemos-baseplate/PinMapping.xlsx
+++ b/wemos-baseplate/wemos-baseplate/PinMapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karij\Documents\Arduino\esp-things\sensemakers-esp32\wemos-baseplate\wemos-baseplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GijsMos\Desktop\sensemakers-esp32\wemos-baseplate\wemos-baseplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99568992-D51F-494F-A8EE-9930E76AA6FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE6FBFB-EF3E-4BAE-A21C-AED7E69E74BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="15120" xr2:uid="{80FB19D3-3E51-444E-B5D4-CA64F88760C8}"/>
+    <workbookView xWindow="38505" yWindow="3900" windowWidth="24990" windowHeight="14565" xr2:uid="{80FB19D3-3E51-444E-B5D4-CA64F88760C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
   <si>
     <t>Gnd</t>
   </si>
@@ -269,52 +269,7 @@
     <t>Vbat</t>
   </si>
   <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>C7,D1,A1</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
-    <t>B7</t>
   </si>
   <si>
     <r>
@@ -357,6 +312,54 @@
   </si>
   <si>
     <t>Row 10</t>
+  </si>
+  <si>
+    <t>A3 (SVN)</t>
+  </si>
+  <si>
+    <t>C5 (D3)</t>
+  </si>
+  <si>
+    <t>C1 (TxD)</t>
+  </si>
+  <si>
+    <t>C2 (RxD)</t>
+  </si>
+  <si>
+    <t>C7,D1,A1 (Gnd)</t>
+  </si>
+  <si>
+    <t>C8 (5V)</t>
+  </si>
+  <si>
+    <t>B2 (SVP)</t>
+  </si>
+  <si>
+    <t>B1 (RST)</t>
+  </si>
+  <si>
+    <t>B7 (D8)</t>
+  </si>
+  <si>
+    <t>B4 (D5)</t>
+  </si>
+  <si>
+    <t>B3 (D0)</t>
+  </si>
+  <si>
+    <t>B6 (D7)</t>
+  </si>
+  <si>
+    <t>B8 (3.3V)</t>
+  </si>
+  <si>
+    <t>B5 (D6)</t>
+  </si>
+  <si>
+    <t>C3 (D1/SCL)(IO34)</t>
+  </si>
+  <si>
+    <t>C4 (D2/SDA)(IO32)</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -543,24 +546,28 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -572,7 +579,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -587,51 +594,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -677,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -692,11 +658,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -764,42 +727,54 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1117,513 +1092,547 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6910671D-0EDD-4780-9ED6-875D2C3AE87F}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" customWidth="1"/>
-    <col min="3" max="3" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B1" s="49" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="49" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="49" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="50"/>
-      <c r="I1" s="49" t="s">
+      <c r="H1" s="47"/>
+      <c r="I1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="50"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="20"/>
-      <c r="B2" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="J2" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="K2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="J1" s="47"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="42"/>
+      <c r="G2" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="23" t="s">
+      <c r="F3" s="48"/>
+      <c r="G3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22" t="s">
+      <c r="I3" s="18"/>
+      <c r="J3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="20"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="47" t="s">
+      <c r="K3" s="17"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="23" t="s">
+      <c r="F4" s="48"/>
+      <c r="G4" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="26" t="s">
+      <c r="I4" s="22"/>
+      <c r="J4" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="20"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="47" t="s">
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="48"/>
+      <c r="G5" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="26" t="s">
+      <c r="I5" s="22"/>
+      <c r="J5" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="47" t="s">
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="27" t="s">
+      <c r="F6" s="48"/>
+      <c r="G6" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="26" t="s">
+      <c r="I6" s="22"/>
+      <c r="J6" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="20"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26" t="s">
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="51"/>
-      <c r="G7" s="23" t="s">
+      <c r="F7" s="48"/>
+      <c r="G7" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="25"/>
-      <c r="J7" s="30" t="s">
+      <c r="I7" s="22"/>
+      <c r="J7" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26" t="s">
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="31" t="s">
+      <c r="F8" s="48"/>
+      <c r="G8" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26" t="s">
+      <c r="I8" s="22"/>
+      <c r="J8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="33" t="s">
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="35" t="s">
+      <c r="E9" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="48"/>
+      <c r="G9" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="36" t="s">
+      <c r="I9" s="22"/>
+      <c r="J9" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="47" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26" t="s">
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="51"/>
-      <c r="G10" s="35" t="s">
+      <c r="F10" s="48"/>
+      <c r="G10" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="36" t="s">
+      <c r="I10" s="22"/>
+      <c r="J10" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="37" t="s">
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="33" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="51"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="38" t="s">
+      <c r="F11" s="48"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="I11" s="25"/>
-      <c r="J11" s="37" t="s">
+      <c r="I11" s="22"/>
+      <c r="J11" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40" t="s">
+      <c r="K11" s="17"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="41" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="41" t="s">
+      <c r="F12" s="48"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="39"/>
-      <c r="J12" s="41" t="s">
+      <c r="I12" s="36"/>
+      <c r="J12" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G14" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="54"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>78</v>
-      </c>
+      <c r="F15" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="54"/>
       <c r="H15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" s="2" t="s">
+      <c r="I15" s="50"/>
+      <c r="J15" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="14" t="s">
-        <v>87</v>
-      </c>
+      <c r="F16" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="48"/>
       <c r="H16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="I16" s="51"/>
+      <c r="J16" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>88</v>
-      </c>
+      <c r="F17" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="48"/>
       <c r="H17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="J17" s="6" t="s">
+      <c r="I17" s="51"/>
+      <c r="J17" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="K17" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="14" t="s">
-        <v>89</v>
-      </c>
+      <c r="F18" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="48"/>
       <c r="H18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="51"/>
+      <c r="J18" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="J18" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>84</v>
-      </c>
+      <c r="G19" s="48"/>
       <c r="H19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J19" s="6" t="s">
+      <c r="I19" s="51"/>
+      <c r="J19" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K19" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>85</v>
-      </c>
+      <c r="F20" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="48"/>
       <c r="H20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" s="6" t="s">
+      <c r="I20" s="51"/>
+      <c r="J20" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K20" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G21" s="14" t="s">
-        <v>86</v>
-      </c>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F21" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="48"/>
       <c r="H21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J21" s="6" t="s">
+      <c r="I21" s="51"/>
+      <c r="J21" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K21" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G22" s="14" t="s">
-        <v>83</v>
-      </c>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F22" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="48"/>
       <c r="H22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J22" s="6" t="s">
+      <c r="I22" s="51"/>
+      <c r="J22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="K22" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G23" s="14" t="s">
-        <v>80</v>
-      </c>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F23" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="48"/>
       <c r="H23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I23" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J23" s="6" t="s">
+      <c r="I23" s="51"/>
+      <c r="J23" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K23" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G24" s="18" t="s">
-        <v>82</v>
-      </c>
+    <row r="24" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="57"/>
       <c r="H24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="J24" s="7" t="s">
+      <c r="I24" s="52"/>
+      <c r="J24" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="J25" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="G14:J14"/>
+  <mergeCells count="16">
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F14:K14"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="I1:J1"/>

</xml_diff>